<commit_message>
Update function, clean 2016-2019 data
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2016.xlsx
+++ b/data/tower_count/tower_count_2016.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6122005-3B11-4182-838F-8ABAAB22C294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,6 +201,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -243,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,9 +285,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,6 +337,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -486,11 +529,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +563,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41801</v>
+        <v>42532</v>
       </c>
       <c r="B2">
         <v>340</v>
@@ -543,7 +586,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41802</v>
+        <v>42533</v>
       </c>
       <c r="B3">
         <v>371</v>
@@ -566,7 +609,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41803</v>
+        <v>42534</v>
       </c>
       <c r="B4">
         <v>416</v>
@@ -589,7 +632,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41804</v>
+        <v>42535</v>
       </c>
       <c r="B5">
         <v>331</v>
@@ -612,7 +655,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41805</v>
+        <v>42536</v>
       </c>
       <c r="B6">
         <v>381</v>
@@ -635,7 +678,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41806</v>
+        <v>42537</v>
       </c>
       <c r="B7">
         <v>486</v>
@@ -658,7 +701,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41807</v>
+        <v>42538</v>
       </c>
       <c r="B8">
         <v>464</v>
@@ -681,7 +724,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41808</v>
+        <v>42539</v>
       </c>
       <c r="B9">
         <v>506</v>
@@ -704,7 +747,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41809</v>
+        <v>42540</v>
       </c>
       <c r="B10">
         <v>517</v>
@@ -727,7 +770,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41810</v>
+        <v>42541</v>
       </c>
       <c r="B11">
         <v>492</v>
@@ -750,7 +793,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41811</v>
+        <v>42542</v>
       </c>
       <c r="B12">
         <v>375</v>
@@ -773,7 +816,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41812</v>
+        <v>42543</v>
       </c>
       <c r="B13">
         <v>406</v>
@@ -796,7 +839,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41813</v>
+        <v>42544</v>
       </c>
       <c r="B14">
         <v>453</v>
@@ -816,7 +859,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41814</v>
+        <v>42545</v>
       </c>
       <c r="B15">
         <v>477</v>
@@ -839,7 +882,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41815</v>
+        <v>42546</v>
       </c>
       <c r="B16">
         <v>552</v>
@@ -859,7 +902,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41816</v>
+        <v>42547</v>
       </c>
       <c r="B17">
         <v>564</v>
@@ -882,7 +925,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41817</v>
+        <v>42548</v>
       </c>
       <c r="B18">
         <v>589</v>
@@ -905,7 +948,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41818</v>
+        <v>42549</v>
       </c>
       <c r="B19">
         <v>468</v>
@@ -928,7 +971,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41819</v>
+        <v>42550</v>
       </c>
       <c r="G20" t="s">
         <v>42</v>
@@ -936,7 +979,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41820</v>
+        <v>42551</v>
       </c>
       <c r="G21" t="s">
         <v>42</v>
@@ -944,7 +987,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41821</v>
+        <v>42552</v>
       </c>
       <c r="B22">
         <v>629</v>
@@ -967,7 +1010,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41822</v>
+        <v>42553</v>
       </c>
       <c r="G23" t="s">
         <v>42</v>
@@ -975,7 +1018,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41823</v>
+        <v>42554</v>
       </c>
       <c r="G24" t="s">
         <v>42</v>
@@ -983,7 +1026,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41824</v>
+        <v>42555</v>
       </c>
       <c r="G25" t="s">
         <v>42</v>
@@ -991,7 +1034,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41825</v>
+        <v>42556</v>
       </c>
       <c r="G26" t="s">
         <v>42</v>
@@ -999,7 +1042,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41826</v>
+        <v>42557</v>
       </c>
       <c r="B27">
         <v>529</v>
@@ -1022,7 +1065,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41827</v>
+        <v>42558</v>
       </c>
       <c r="B28">
         <v>379</v>
@@ -1045,7 +1088,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41828</v>
+        <v>42559</v>
       </c>
       <c r="G29" t="s">
         <v>42</v>
@@ -1053,7 +1096,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41829</v>
+        <v>42560</v>
       </c>
       <c r="G30" t="s">
         <v>42</v>
@@ -1061,7 +1104,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41830</v>
+        <v>42561</v>
       </c>
       <c r="B31">
         <v>506</v>
@@ -1084,7 +1127,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41831</v>
+        <v>42562</v>
       </c>
       <c r="B32">
         <v>552</v>
@@ -1107,7 +1150,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41832</v>
+        <v>42563</v>
       </c>
       <c r="B33">
         <v>532</v>
@@ -1130,7 +1173,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41833</v>
+        <v>42564</v>
       </c>
       <c r="B34">
         <v>545</v>
@@ -1153,7 +1196,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41834</v>
+        <v>42565</v>
       </c>
       <c r="G35" t="s">
         <v>42</v>
@@ -1161,7 +1204,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41835</v>
+        <v>42566</v>
       </c>
       <c r="G36" t="s">
         <v>42</v>
@@ -1169,7 +1212,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41836</v>
+        <v>42567</v>
       </c>
       <c r="B37">
         <v>550</v>
@@ -1192,7 +1235,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41837</v>
+        <v>42568</v>
       </c>
       <c r="B38">
         <v>589</v>
@@ -1212,7 +1255,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41838</v>
+        <v>42569</v>
       </c>
       <c r="G39" t="s">
         <v>42</v>
@@ -1220,7 +1263,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41839</v>
+        <v>42570</v>
       </c>
       <c r="B40">
         <v>520</v>
@@ -1243,7 +1286,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41840</v>
+        <v>42571</v>
       </c>
       <c r="B41">
         <v>352</v>
@@ -1263,7 +1306,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41841</v>
+        <v>42572</v>
       </c>
       <c r="B42">
         <v>482</v>
@@ -1283,7 +1326,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41842</v>
+        <v>42573</v>
       </c>
       <c r="B43">
         <v>435</v>
@@ -1303,7 +1346,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41843</v>
+        <v>42574</v>
       </c>
       <c r="B44">
         <v>470</v>
@@ -1323,7 +1366,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41844</v>
+        <v>42575</v>
       </c>
       <c r="B45">
         <v>476</v>
@@ -1343,7 +1386,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41845</v>
+        <v>42576</v>
       </c>
       <c r="B46">
         <v>535</v>
@@ -1363,7 +1406,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41846</v>
+        <v>42577</v>
       </c>
       <c r="G47" t="s">
         <v>42</v>
@@ -1371,7 +1414,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41847</v>
+        <v>42578</v>
       </c>
       <c r="B48">
         <v>581</v>
@@ -1391,7 +1434,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41848</v>
+        <v>42579</v>
       </c>
       <c r="B49">
         <v>633</v>
@@ -1411,7 +1454,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41849</v>
+        <v>42580</v>
       </c>
       <c r="G50" t="s">
         <v>42</v>
@@ -1419,7 +1462,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41850</v>
+        <v>42581</v>
       </c>
       <c r="B51">
         <v>625</v>
@@ -1439,7 +1482,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41851</v>
+        <v>42582</v>
       </c>
       <c r="B52">
         <v>625</v>
@@ -1459,7 +1502,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41852</v>
+        <v>42583</v>
       </c>
       <c r="B53">
         <v>608</v>
@@ -1479,7 +1522,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41853</v>
+        <v>42584</v>
       </c>
       <c r="B54">
         <v>594</v>
@@ -1499,7 +1542,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41854</v>
+        <v>42585</v>
       </c>
       <c r="B55">
         <v>620</v>
@@ -1523,7 +1566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1535,7 +1578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>